<commit_message>
re-ran all fits and generated first drafts of paper figs
</commit_message>
<xml_diff>
--- a/N_xi Fits/Results/Results (PW=True, rho=0.7)/N_xi Fitted Parameters (rho=0.7, PW=True).xlsx
+++ b/N_xi Fits/Results/Results (PW=True, rho=0.7)/N_xi Fitted Parameters (rho=0.7, PW=True).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O49"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,7 +513,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -521,50 +521,50 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>AC6rearSOAEwfB1.mat</t>
+          <t>ALrearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1232.77587890625</v>
+        <v>2804.69970703125</v>
       </c>
       <c r="E2" t="n">
-        <v>19.19449889239234</v>
+        <v>192.029908346541</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4020660705550928</v>
+        <v>2.293935380724255</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01557014476096189</v>
+        <v>0.06846719021830791</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0003261469318428067</v>
+        <v>0.0008178898350413296</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5481487529989877</v>
+        <v>0.4745592015199314</v>
       </c>
       <c r="J2" t="n">
-        <v>0.01042907641903129</v>
+        <v>0.005308918663555654</v>
       </c>
       <c r="K2" t="n">
-        <v>7.753878938777798e-05</v>
+        <v>9.004317649699155e-05</v>
       </c>
       <c r="L2" t="n">
-        <v>0.03591836734693878</v>
+        <v>0.1656235827664399</v>
       </c>
       <c r="M2" t="n">
-        <v>44.279296875</v>
+        <v>464.5244140625</v>
       </c>
       <c r="N2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O2" t="n">
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -572,50 +572,50 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>AC6rearSOAEwfB1.mat</t>
+          <t>ALrearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2164.0869140625</v>
+        <v>2944.66552734375</v>
       </c>
       <c r="E3" t="n">
-        <v>22.79809024014023</v>
+        <v>209.5765669696959</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5652887685931292</v>
+        <v>1.748555249764147</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0105347387353047</v>
+        <v>0.07117160337009328</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0002612135237821614</v>
+        <v>0.0005938043670927338</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5729785674750908</v>
+        <v>0.7018140074405008</v>
       </c>
       <c r="J3" t="n">
-        <v>0.01260321433621463</v>
+        <v>0.005559929714109686</v>
       </c>
       <c r="K3" t="n">
-        <v>7.921778519257061e-05</v>
+        <v>9.748412695513171e-05</v>
       </c>
       <c r="L3" t="n">
-        <v>0.02394557823129252</v>
+        <v>0.1736054421768707</v>
       </c>
       <c r="M3" t="n">
-        <v>51.8203125</v>
+        <v>511.2099609375</v>
       </c>
       <c r="N3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O3" t="n">
-        <v>59</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -623,101 +623,101 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>AC6rearSOAEwfB1.mat</t>
+          <t>ALrearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3709.09423828125</v>
+        <v>3865.2099609375</v>
       </c>
       <c r="E4" t="n">
-        <v>32.59504692072368</v>
+        <v>317.9871936224826</v>
       </c>
       <c r="F4" t="n">
-        <v>0.869598868040044</v>
+        <v>1.900514802786706</v>
       </c>
       <c r="G4" t="n">
-        <v>0.008787872409472085</v>
+        <v>0.08226906088831337</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0002344504647698048</v>
+        <v>0.0004916976883516412</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7271641617155876</v>
+        <v>0.7286166575899398</v>
       </c>
       <c r="J4" t="n">
-        <v>0.01688621332754525</v>
+        <v>0.003840604266019119</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0001530949053136054</v>
+        <v>8.524685893176866e-05</v>
       </c>
       <c r="L4" t="n">
-        <v>0.02195011337868481</v>
+        <v>0.2145124716553288</v>
       </c>
       <c r="M4" t="n">
-        <v>81.4150390625</v>
+        <v>829.1357421875</v>
       </c>
       <c r="N4" t="n">
         <v>13</v>
       </c>
       <c r="O4" t="n">
-        <v>79</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AC6rearSOAEwfB1.mat</t>
+          <t>JIrearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4505.82275390625</v>
+        <v>2341.73583984375</v>
       </c>
       <c r="E5" t="n">
-        <v>-4505.82275390625</v>
+        <v>453.3055553336419</v>
       </c>
       <c r="F5" t="n">
-        <v>-4505.82275390625</v>
+        <v>1.525282303754003</v>
       </c>
       <c r="G5" t="n">
-        <v>-1</v>
+        <v>0.1935767252739695</v>
       </c>
       <c r="H5" t="n">
-        <v>-1</v>
+        <v>0.0006513468674826176</v>
       </c>
       <c r="I5" t="n">
-        <v>-1</v>
+        <v>1.442049229287201</v>
       </c>
       <c r="J5" t="n">
-        <v>-1</v>
+        <v>0.006173817720904584</v>
       </c>
       <c r="K5" t="n">
-        <v>-1</v>
+        <v>9.917860158785643e-05</v>
       </c>
       <c r="L5" t="n">
-        <v>0.00598639455782313</v>
+        <v>0.563718820861678</v>
       </c>
       <c r="M5" t="n">
-        <v>26.9736328125</v>
+        <v>1320.08056640625</v>
       </c>
       <c r="N5" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="O5" t="n">
-        <v>128</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -725,50 +725,50 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ACsb4rearSOAEwf1.mat</t>
+          <t>JIrearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>963.61083984375</v>
+        <v>4048.2421875</v>
       </c>
       <c r="E6" t="n">
-        <v>14.42788619691109</v>
+        <v>460.7085682338297</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6102154343158137</v>
+        <v>2.43794400350096</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01497273131469814</v>
+        <v>0.113804596389116</v>
       </c>
       <c r="H6" t="n">
-        <v>0.000633259204944976</v>
+        <v>0.0006022228637972169</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2507286482420771</v>
+        <v>1.576540459646145</v>
       </c>
       <c r="J6" t="n">
-        <v>0.008703974219404078</v>
+        <v>0.01301713823293699</v>
       </c>
       <c r="K6" t="n">
-        <v>3.311905015838076e-05</v>
+        <v>9.79501214349092e-05</v>
       </c>
       <c r="L6" t="n">
-        <v>0.02494331065759637</v>
+        <v>0.3751473922902495</v>
       </c>
       <c r="M6" t="n">
-        <v>24.03564453125</v>
+        <v>1518.6875</v>
       </c>
       <c r="N6" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="O6" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -776,454 +776,458 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ACsb4rearSOAEwf1.mat</t>
+          <t>JIrearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3025.4150390625</v>
+        <v>5840.88134765625</v>
       </c>
       <c r="E7" t="n">
-        <v>86.21159085641949</v>
+        <v>431.7057284501211</v>
       </c>
       <c r="F7" t="n">
-        <v>7.800272027433216</v>
+        <v>3.988964057316069</v>
       </c>
       <c r="G7" t="n">
-        <v>0.02849578974894443</v>
+        <v>0.07391105943683483</v>
       </c>
       <c r="H7" t="n">
-        <v>0.002578248579689193</v>
+        <v>0.0006829387244643663</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1152145194211855</v>
+        <v>0.8655601461725978</v>
       </c>
       <c r="J7" t="n">
-        <v>0.005293779720022995</v>
+        <v>0.009970941292781867</v>
       </c>
       <c r="K7" t="n">
-        <v>7.125666383919681e-06</v>
+        <v>9.860525401897546e-05</v>
       </c>
       <c r="L7" t="n">
-        <v>0.02195011337868481</v>
+        <v>0.2035374149659864</v>
       </c>
       <c r="M7" t="n">
-        <v>66.408203125</v>
+        <v>1188.837890625</v>
       </c>
       <c r="N7" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="O7" t="n">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ACsb4rearSOAEwf1.mat</t>
+          <t>LSrearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3154.6142578125</v>
+        <v>732.12890625</v>
       </c>
       <c r="E8" t="n">
-        <v>23.79891661203681</v>
+        <v>236.8866940192555</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7782374417737637</v>
+        <v>0.6585848234327349</v>
       </c>
       <c r="G8" t="n">
-        <v>0.007544160606355614</v>
+        <v>0.3235587230568463</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0002466981311095119</v>
+        <v>0.0008995476313126858</v>
       </c>
       <c r="I8" t="n">
-        <v>0.5803310018832893</v>
+        <v>1.106820063056558</v>
       </c>
       <c r="J8" t="n">
-        <v>0.02105456070573184</v>
+        <v>0.003414069295155298</v>
       </c>
       <c r="K8" t="n">
-        <v>4.97851583740326e-05</v>
+        <v>9.81741299794309e-05</v>
       </c>
       <c r="L8" t="n">
-        <v>0.01795918367346939</v>
+        <v>0.9049433106575964</v>
       </c>
       <c r="M8" t="n">
-        <v>56.654296875</v>
+        <v>662.53515625</v>
       </c>
       <c r="N8" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O8" t="n">
-        <v>82</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ACsb4rearSOAEwf1.mat</t>
+          <t>LSrearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>3951.3427734375</v>
+        <v>2228.6865234375</v>
       </c>
       <c r="E9" t="n">
-        <v>29.11413947809145</v>
+        <v>294.1251217324845</v>
       </c>
       <c r="F9" t="n">
-        <v>4.269459745703388</v>
+        <v>1.391416566883124</v>
       </c>
       <c r="G9" t="n">
-        <v>0.007368163469342191</v>
+        <v>0.1319724055578841</v>
       </c>
       <c r="H9" t="n">
-        <v>0.001080508574048396</v>
+        <v>0.0006243213445455842</v>
       </c>
       <c r="I9" t="n">
-        <v>0.2860106714308474</v>
+        <v>1.400585875541453</v>
       </c>
       <c r="J9" t="n">
-        <v>0.02312188080443922</v>
+        <v>0.009180777177074504</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0001083651147079655</v>
+        <v>9.977511028456379e-05</v>
       </c>
       <c r="L9" t="n">
-        <v>0.007981859410430839</v>
+        <v>0.4020861678004535</v>
       </c>
       <c r="M9" t="n">
-        <v>31.5390625</v>
+        <v>896.1240234375</v>
       </c>
       <c r="N9" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="O9" t="n">
-        <v>104</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ACsb24rearSOAEwfA1.mat</t>
+          <t>TH13RearwaveformSOAE.mat</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2174.853515625</v>
+        <v>904.39453125</v>
       </c>
       <c r="E10" t="n">
-        <v>23.4534936045619</v>
+        <v>203.5714746263814</v>
       </c>
       <c r="F10" t="n">
-        <v>0.324283836652215</v>
+        <v>0.6983354689746077</v>
       </c>
       <c r="G10" t="n">
-        <v>0.01078394173955294</v>
+        <v>0.2250914480265787</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0001491060590161281</v>
+        <v>0.0007721579961451229</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8428557812150416</v>
+        <v>0.8504783020152371</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0110450441254052</v>
+        <v>0.002972412431776154</v>
       </c>
       <c r="K10" t="n">
-        <v>8.211091894936803e-05</v>
+        <v>7.220259389062832e-05</v>
       </c>
       <c r="L10" t="n">
-        <v>0.03691609977324263</v>
+        <v>0.5936507936507937</v>
       </c>
       <c r="M10" t="n">
-        <v>80.287109375</v>
+        <v>536.89453125</v>
       </c>
       <c r="N10" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="O10" t="n">
-        <v>64</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>ACsb24rearSOAEwfA1.mat</t>
+          <t>TH13RearwaveformSOAE.mat</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2503.23486328125</v>
+        <v>1518.0908203125</v>
       </c>
       <c r="E11" t="n">
-        <v>23.34635448375462</v>
+        <v>390.4677566393477</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4026351925600824</v>
+        <v>1.125929233793116</v>
       </c>
       <c r="G11" t="n">
-        <v>0.009326473846386164</v>
+        <v>0.2572097475426204</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0001608459511594955</v>
+        <v>0.0007416744892517979</v>
       </c>
       <c r="I11" t="n">
-        <v>0.7475239048208392</v>
+        <v>0.9849243512522977</v>
       </c>
       <c r="J11" t="n">
-        <v>0.01153957454766842</v>
+        <v>0.002639614546769247</v>
       </c>
       <c r="K11" t="n">
-        <v>9.349435167831297e-05</v>
+        <v>9.734134148774066e-05</v>
       </c>
       <c r="L11" t="n">
-        <v>0.02993197278911565</v>
+        <v>0.6604988662131519</v>
       </c>
       <c r="M11" t="n">
-        <v>74.9267578125</v>
+        <v>1002.697265625</v>
       </c>
       <c r="N11" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O11" t="n">
-        <v>74</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ACsb24rearSOAEwfA1.mat</t>
+          <t>TH13RearwaveformSOAE.mat</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3111.5478515625</v>
+        <v>2040.27099609375</v>
       </c>
       <c r="E12" t="n">
-        <v>20.80581232456634</v>
+        <v>245.2428450037529</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3493360247505561</v>
+        <v>1.055976179172113</v>
       </c>
       <c r="G12" t="n">
-        <v>0.006686643856085473</v>
+        <v>0.1202011132213752</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0001122708187100941</v>
+        <v>0.0005175666277635948</v>
       </c>
       <c r="I12" t="n">
-        <v>0.6426101108015128</v>
+        <v>1.079991055365171</v>
       </c>
       <c r="J12" t="n">
-        <v>0.01165106352218021</v>
+        <v>0.00491531535775632</v>
       </c>
       <c r="K12" t="n">
-        <v>2.067896538439963e-05</v>
+        <v>9.938279830330118e-05</v>
       </c>
       <c r="L12" t="n">
-        <v>0.01795918367346939</v>
+        <v>0.3452154195011338</v>
       </c>
       <c r="M12" t="n">
-        <v>55.880859375</v>
+        <v>704.3330078125</v>
       </c>
       <c r="N12" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="O12" t="n">
-        <v>85</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ACsb24rearSOAEwfA1.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3477.6123046875</v>
+        <v>8016.15074024226</v>
       </c>
       <c r="E13" t="n">
-        <v>26.33905053492246</v>
+        <v>40.61349559244912</v>
       </c>
       <c r="F13" t="n">
-        <v>0.4955630824542408</v>
+        <v>1.947685096238222</v>
       </c>
       <c r="G13" t="n">
-        <v>0.007573889274379394</v>
+        <v>0.00506645856702312</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0001425009572764243</v>
+        <v>0.0002429701186207185</v>
       </c>
       <c r="I13" t="n">
-        <v>0.5175314282102106</v>
+        <v>0.2193598501738097</v>
       </c>
       <c r="J13" t="n">
-        <v>0.01060122415688905</v>
+        <v>0.009568152762600875</v>
       </c>
       <c r="K13" t="n">
-        <v>1.164977127779359e-05</v>
+        <v>2.688204889732216e-05</v>
       </c>
       <c r="L13" t="n">
-        <v>0.01696145124716553</v>
+        <v>0.015</v>
       </c>
       <c r="M13" t="n">
-        <v>58.9853515625</v>
+        <v>120.2422611036339</v>
       </c>
       <c r="N13" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="O13" t="n">
-        <v>81</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Anole</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ACsb30learSOAEwfA2.mat</t>
+          <t>Owl2R1.mat</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1798.0224609375</v>
+        <v>8452.220726783311</v>
       </c>
       <c r="E14" t="n">
-        <v>13.78434451613604</v>
+        <v>28.51385937434651</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2604784346755091</v>
+        <v>0.6697854667596558</v>
       </c>
       <c r="G14" t="n">
-        <v>0.007666391725133845</v>
+        <v>0.003373534636168703</v>
       </c>
       <c r="H14" t="n">
-        <v>0.0001448693997625002</v>
+        <v>7.924372640165991e-05</v>
       </c>
       <c r="I14" t="n">
-        <v>0.5731722619181375</v>
+        <v>0.3761173385972644</v>
       </c>
       <c r="J14" t="n">
-        <v>0.01137051994052748</v>
+        <v>0.009281475667517405</v>
       </c>
       <c r="K14" t="n">
-        <v>3.41350606875744e-05</v>
+        <v>8.592730953287137e-06</v>
       </c>
       <c r="L14" t="n">
-        <v>0.02394557823129252</v>
+        <v>0.011</v>
       </c>
       <c r="M14" t="n">
-        <v>43.0546875</v>
+        <v>92.97442799461642</v>
       </c>
       <c r="N14" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="O14" t="n">
-        <v>103</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>tokay_GG1rearSOAEwf.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>3213.83056640625</v>
+        <v>7924.629878869448</v>
       </c>
       <c r="E15" t="n">
-        <v>-3213.83056640625</v>
+        <v>49.27568818282902</v>
       </c>
       <c r="F15" t="n">
-        <v>-3213.83056640625</v>
+        <v>2.135507926358779</v>
       </c>
       <c r="G15" t="n">
-        <v>-1</v>
+        <v>0.006218042853234029</v>
       </c>
       <c r="H15" t="n">
-        <v>-1</v>
+        <v>0.0002694773079627332</v>
       </c>
       <c r="I15" t="n">
-        <v>-1</v>
+        <v>0.2341146159854675</v>
       </c>
       <c r="J15" t="n">
-        <v>-1</v>
+        <v>0.0101626015394115</v>
       </c>
       <c r="K15" t="n">
-        <v>-1</v>
+        <v>2.590957006433445e-05</v>
       </c>
       <c r="L15" t="n">
-        <v>0.004988662131519274</v>
+        <v>0.019</v>
       </c>
       <c r="M15" t="n">
-        <v>16.03271484375</v>
-      </c>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
+        <v>150.5679676985195</v>
+      </c>
+      <c r="N15" t="n">
+        <v>7</v>
+      </c>
+      <c r="O15" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1231,46 +1235,50 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>tokay_GG2rearSOAEwf.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1566.54052734375</v>
+        <v>7537.012113055182</v>
       </c>
       <c r="E16" t="n">
-        <v>-1566.54052734375</v>
+        <v>41.24202729640625</v>
       </c>
       <c r="F16" t="n">
-        <v>-1566.54052734375</v>
+        <v>1.607541971282317</v>
       </c>
       <c r="G16" t="n">
-        <v>-1</v>
+        <v>0.005471933264505329</v>
       </c>
       <c r="H16" t="n">
-        <v>-1</v>
+        <v>0.0002132863722612074</v>
       </c>
       <c r="I16" t="n">
-        <v>-1</v>
+        <v>0.1202287246651158</v>
       </c>
       <c r="J16" t="n">
-        <v>-1</v>
+        <v>0.004924720792896847</v>
       </c>
       <c r="K16" t="n">
-        <v>-1</v>
+        <v>4.236747888474907e-06</v>
       </c>
       <c r="L16" t="n">
-        <v>0.008979591836734694</v>
+        <v>0.017</v>
       </c>
       <c r="M16" t="n">
-        <v>14.06689453125</v>
-      </c>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
+        <v>128.1292059219381</v>
+      </c>
+      <c r="N16" t="n">
+        <v>5</v>
+      </c>
+      <c r="O16" t="n">
+        <v>107</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1278,93 +1286,101 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>tokay_GG2rearSOAEwf.mat</t>
+          <t>Owl7L1.mat</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3176.1474609375</v>
+        <v>8855.989232839838</v>
       </c>
       <c r="E17" t="n">
-        <v>32.65891660494093</v>
+        <v>45.94627716014756</v>
       </c>
       <c r="F17" t="n">
-        <v>0.5299094178031407</v>
+        <v>0.7409534265507758</v>
       </c>
       <c r="G17" t="n">
-        <v>0.01028255677880303</v>
+        <v>0.005188158651974109</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0001668403071080106</v>
+        <v>8.366692947222286e-05</v>
       </c>
       <c r="I17" t="n">
-        <v>0.3860613845199615</v>
+        <v>0.329155188085536</v>
       </c>
       <c r="J17" t="n">
-        <v>0.005745152752552131</v>
+        <v>0.005686992660103132</v>
       </c>
       <c r="K17" t="n">
-        <v>1.684872627679584e-05</v>
+        <v>4.76387862993541e-06</v>
       </c>
       <c r="L17" t="n">
-        <v>0.02594104308390023</v>
+        <v>0.016</v>
       </c>
       <c r="M17" t="n">
-        <v>82.392578125</v>
-      </c>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
+        <v>141.6958277254374</v>
+      </c>
+      <c r="N17" t="n">
+        <v>7</v>
+      </c>
+      <c r="O17" t="n">
+        <v>107</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>tokay_GG2rearSOAEwf.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>3875.9765625</v>
+        <v>6029.296875</v>
       </c>
       <c r="E18" t="n">
-        <v>-3875.9765625</v>
+        <v>65.13278592399242</v>
       </c>
       <c r="F18" t="n">
-        <v>-3875.9765625</v>
+        <v>1.071674204893664</v>
       </c>
       <c r="G18" t="n">
-        <v>-1</v>
+        <v>0.0108027166806233</v>
       </c>
       <c r="H18" t="n">
-        <v>-1</v>
+        <v>0.0001777444745401865</v>
       </c>
       <c r="I18" t="n">
-        <v>-1</v>
+        <v>0.1595743802840819</v>
       </c>
       <c r="J18" t="n">
-        <v>-1</v>
+        <v>0.002432609131846734</v>
       </c>
       <c r="K18" t="n">
-        <v>-1</v>
+        <v>3.703339274596615e-06</v>
       </c>
       <c r="L18" t="n">
-        <v>0.004988662131519274</v>
+        <v>0.0309297052154195</v>
       </c>
       <c r="M18" t="n">
-        <v>19.3359375</v>
-      </c>
-      <c r="N18" t="inlineStr"/>
-      <c r="O18" t="inlineStr"/>
+        <v>186.484375</v>
+      </c>
+      <c r="N18" t="n">
+        <v>6</v>
+      </c>
+      <c r="O18" t="n">
+        <v>85</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1372,46 +1388,50 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>tokay_GG3rearSOAEwf.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>1108.9599609375</v>
+        <v>8101.86767578125</v>
       </c>
       <c r="E19" t="n">
-        <v>17.88548469707924</v>
+        <v>42.88976950158132</v>
       </c>
       <c r="F19" t="n">
-        <v>0.2304691732170706</v>
+        <v>0.5339612227321732</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0161281609139063</v>
+        <v>0.005293812639003084</v>
       </c>
       <c r="H19" t="n">
-        <v>0.0002078246116498516</v>
+        <v>6.590594219754202e-05</v>
       </c>
       <c r="I19" t="n">
-        <v>0.212880807158168</v>
+        <v>0.2343742302548313</v>
       </c>
       <c r="J19" t="n">
-        <v>0.002686251438567211</v>
+        <v>0.003114817991482391</v>
       </c>
       <c r="K19" t="n">
-        <v>4.839303522408686e-06</v>
+        <v>1.575543687285235e-06</v>
       </c>
       <c r="L19" t="n">
-        <v>0.04290249433106576</v>
+        <v>0.01696145124716553</v>
       </c>
       <c r="M19" t="n">
-        <v>47.5771484375</v>
-      </c>
-      <c r="N19" t="inlineStr"/>
-      <c r="O19" t="inlineStr"/>
+        <v>137.41943359375</v>
+      </c>
+      <c r="N19" t="n">
+        <v>6</v>
+      </c>
+      <c r="O19" t="n">
+        <v>103</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1419,93 +1439,101 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>tokay_GG3rearSOAEwf.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>3133.0810546875</v>
+        <v>8489.46533203125</v>
       </c>
       <c r="E20" t="n">
-        <v>34.4536522618348</v>
+        <v>84.66071131926938</v>
       </c>
       <c r="F20" t="n">
-        <v>1.986366317493123</v>
+        <v>1.774116051566171</v>
       </c>
       <c r="G20" t="n">
-        <v>0.01099673186248649</v>
+        <v>0.009972443258568895</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0006339977430591075</v>
+        <v>0.0002089785377734364</v>
       </c>
       <c r="I20" t="n">
-        <v>0.273525989274533</v>
+        <v>0.4585553030598876</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0115941638859354</v>
+        <v>0.008247983403926554</v>
       </c>
       <c r="K20" t="n">
-        <v>4.20371812218127e-05</v>
+        <v>5.106006724473076e-05</v>
       </c>
       <c r="L20" t="n">
-        <v>0.01596371882086168</v>
+        <v>0.02693877551020408</v>
       </c>
       <c r="M20" t="n">
-        <v>50.015625</v>
-      </c>
-      <c r="N20" t="inlineStr"/>
-      <c r="O20" t="inlineStr"/>
+        <v>228.69580078125</v>
+      </c>
+      <c r="N20" t="n">
+        <v>10</v>
+      </c>
+      <c r="O20" t="n">
+        <v>69</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>tokay_GG4rearSOAEwf.mat</t>
+          <t>TAG6rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1103.57666015625</v>
+        <v>9856.82373046875</v>
       </c>
       <c r="E21" t="n">
-        <v>16.59963013684566</v>
+        <v>68.40073712685779</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2699366345225815</v>
+        <v>1.257538133271619</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0150416647398971</v>
+        <v>0.006939429880989151</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0002446016160620528</v>
+        <v>0.0001275804628000399</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2639707474729727</v>
+        <v>0.1465530753737588</v>
       </c>
       <c r="J21" t="n">
-        <v>0.003975699661767767</v>
+        <v>0.002613693385808118</v>
       </c>
       <c r="K21" t="n">
-        <v>1.058877720420292e-05</v>
+        <v>2.363542349859551e-06</v>
       </c>
       <c r="L21" t="n">
-        <v>0.03591836734693878</v>
+        <v>0.02195011337868481</v>
       </c>
       <c r="M21" t="n">
-        <v>39.638671875</v>
-      </c>
-      <c r="N21" t="inlineStr"/>
-      <c r="O21" t="inlineStr"/>
+        <v>216.3583984375</v>
+      </c>
+      <c r="N21" t="n">
+        <v>4</v>
+      </c>
+      <c r="O21" t="n">
+        <v>113</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1513,88 +1541,96 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>tokay_GG4rearSOAEwf.mat</t>
+          <t>TAG9rearSOAEwf2.mat</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>2287.90283203125</v>
+        <v>6976.7578125</v>
       </c>
       <c r="E22" t="n">
-        <v>27.19560419212578</v>
+        <v>57.14257245516263</v>
       </c>
       <c r="F22" t="n">
-        <v>1.985760599208237</v>
+        <v>1.356035664374745</v>
       </c>
       <c r="G22" t="n">
-        <v>0.0118866954537492</v>
+        <v>0.008190419388327109</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0008679392198860279</v>
+        <v>0.0001943647322750957</v>
       </c>
       <c r="I22" t="n">
-        <v>0.2093830686897698</v>
+        <v>0.4757257971684064</v>
       </c>
       <c r="J22" t="n">
-        <v>0.009744833640685537</v>
+        <v>0.01168325743842804</v>
       </c>
       <c r="K22" t="n">
-        <v>8.484125734387891e-06</v>
+        <v>4.552811302754335e-05</v>
       </c>
       <c r="L22" t="n">
-        <v>0.01197278911564626</v>
+        <v>0.02793650793650794</v>
       </c>
       <c r="M22" t="n">
-        <v>27.392578125</v>
-      </c>
-      <c r="N22" t="inlineStr"/>
-      <c r="O22" t="inlineStr"/>
+        <v>194.90625</v>
+      </c>
+      <c r="N22" t="n">
+        <v>10</v>
+      </c>
+      <c r="O22" t="n">
+        <v>73</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Tokay</t>
+          <t>Owl</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>tokay_GG4rearSOAEwf.mat</t>
+          <t>owl_TAG4learSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3159.99755859375</v>
+        <v>5770.8984375</v>
       </c>
       <c r="E23" t="n">
-        <v>30.57525290321044</v>
+        <v>70.97890720788696</v>
       </c>
       <c r="F23" t="n">
-        <v>2.636495221700664</v>
+        <v>1.582891169500671</v>
       </c>
       <c r="G23" t="n">
-        <v>0.009675720419485679</v>
+        <v>0.01229945527141101</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0008343345755222504</v>
+        <v>0.0002742885161892387</v>
       </c>
       <c r="I23" t="n">
-        <v>0.228497572572266</v>
+        <v>0.3512023180130218</v>
       </c>
       <c r="J23" t="n">
-        <v>0.01192558354788435</v>
+        <v>0.007056195418087159</v>
       </c>
       <c r="K23" t="n">
-        <v>3.322685957146147e-05</v>
+        <v>4.307443167580436e-05</v>
       </c>
       <c r="L23" t="n">
-        <v>0.0109750566893424</v>
+        <v>0.03691609977324263</v>
       </c>
       <c r="M23" t="n">
-        <v>34.68115234375</v>
-      </c>
-      <c r="N23" t="inlineStr"/>
-      <c r="O23" t="inlineStr"/>
+        <v>213.0390625</v>
+      </c>
+      <c r="N23" t="n">
+        <v>9</v>
+      </c>
+      <c r="O23" t="n">
+        <v>58</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1603,48 +1639,48 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>owl_TAG4learSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>8016.15074024226</v>
+        <v>7175.93994140625</v>
       </c>
       <c r="E24" t="n">
-        <v>41.06135205150375</v>
+        <v>148.6245472243766</v>
       </c>
       <c r="F24" t="n">
-        <v>1.705022362807809</v>
+        <v>1.934658271394006</v>
       </c>
       <c r="G24" t="n">
-        <v>0.005122327833154346</v>
+        <v>0.02071150935458512</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0002126983907935195</v>
+        <v>0.0002696034647991878</v>
       </c>
       <c r="I24" t="n">
-        <v>0.2176939461975896</v>
+        <v>1.321089240351001</v>
       </c>
       <c r="J24" t="n">
-        <v>0.008367803178887294</v>
+        <v>0.02452738531611359</v>
       </c>
       <c r="K24" t="n">
-        <v>2.304091638658976e-05</v>
+        <v>8.892517160604191e-05</v>
       </c>
       <c r="L24" t="n">
-        <v>0.018</v>
+        <v>0.06285714285714286</v>
       </c>
       <c r="M24" t="n">
-        <v>144.2907133243607</v>
+        <v>451.0590820312501</v>
       </c>
       <c r="N24" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="O24" t="n">
-        <v>124</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25">
@@ -1654,819 +1690,811 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Owl2R1.mat</t>
+          <t>owl_TAG4learSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>8452.220726783311</v>
+        <v>9630.72509765625</v>
       </c>
       <c r="E25" t="n">
-        <v>28.81489078896067</v>
+        <v>138.9773127809055</v>
       </c>
       <c r="F25" t="n">
-        <v>0.6609719073112509</v>
+        <v>1.582711385268075</v>
       </c>
       <c r="G25" t="n">
-        <v>0.003409150295572895</v>
+        <v>0.01443061777505489</v>
       </c>
       <c r="H25" t="n">
-        <v>7.82009756580031e-05</v>
+        <v>0.0001643397946903548</v>
       </c>
       <c r="I25" t="n">
-        <v>0.3727415219660906</v>
+        <v>0.7275152777757518</v>
       </c>
       <c r="J25" t="n">
-        <v>0.009078470908050003</v>
+        <v>0.00657993205218849</v>
       </c>
       <c r="K25" t="n">
-        <v>9.427831193301617e-06</v>
+        <v>6.650976815346274e-05</v>
       </c>
       <c r="L25" t="n">
-        <v>0.013</v>
+        <v>0.03791383219954648</v>
       </c>
       <c r="M25" t="n">
-        <v>109.878869448183</v>
+        <v>365.1376953125</v>
       </c>
       <c r="N25" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="O25" t="n">
-        <v>126</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>AC6rearSOAEwfB1.mat</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>7924.629878869448</v>
+        <v>1232.77587890625</v>
       </c>
       <c r="E26" t="n">
-        <v>52.36770800092386</v>
+        <v>19.01704570077373</v>
       </c>
       <c r="F26" t="n">
-        <v>2.383280116897357</v>
+        <v>0.3304146568641991</v>
       </c>
       <c r="G26" t="n">
-        <v>0.006608221305143755</v>
+        <v>0.01542619873260835</v>
       </c>
       <c r="H26" t="n">
-        <v>0.000300743397903318</v>
+        <v>0.0002680249204400003</v>
       </c>
       <c r="I26" t="n">
-        <v>0.2226660108972733</v>
+        <v>0.5517581986736415</v>
       </c>
       <c r="J26" t="n">
-        <v>0.01026577288604862</v>
+        <v>0.009096847025078854</v>
       </c>
       <c r="K26" t="n">
-        <v>3.853963936335414e-05</v>
+        <v>6.57365532865058e-05</v>
       </c>
       <c r="L26" t="n">
-        <v>0.1</v>
+        <v>0.04290249433106576</v>
       </c>
       <c r="M26" t="n">
-        <v>792.4629878869448</v>
+        <v>52.88916015625</v>
       </c>
       <c r="N26" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="O26" t="n">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>AC6rearSOAEwfB1.mat</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>7537.012113055182</v>
+        <v>2164.0869140625</v>
       </c>
       <c r="E27" t="n">
-        <v>43.59888606043902</v>
+        <v>22.58497929835468</v>
       </c>
       <c r="F27" t="n">
-        <v>2.839057408710878</v>
+        <v>0.4561736835537722</v>
       </c>
       <c r="G27" t="n">
-        <v>0.005784637918376106</v>
+        <v>0.01043626258797405</v>
       </c>
       <c r="H27" t="n">
-        <v>0.0003766820811914612</v>
+        <v>0.0002107926814720334</v>
       </c>
       <c r="I27" t="n">
-        <v>0.115241612360115</v>
+        <v>0.5766844829667737</v>
       </c>
       <c r="J27" t="n">
-        <v>0.00680915191574023</v>
+        <v>0.01084043557384561</v>
       </c>
       <c r="K27" t="n">
-        <v>5.302375782591717e-06</v>
+        <v>6.635500285588294e-05</v>
       </c>
       <c r="L27" t="n">
-        <v>0.011</v>
+        <v>0.02893424036281179</v>
       </c>
       <c r="M27" t="n">
-        <v>82.90713324360699</v>
+        <v>62.6162109375</v>
       </c>
       <c r="N27" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="O27" t="n">
-        <v>107</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Owl7L1.mat</t>
+          <t>AC6rearSOAEwfB1.mat</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>8855.989232839838</v>
+        <v>3709.09423828125</v>
       </c>
       <c r="E28" t="n">
-        <v>47.44399045684062</v>
+        <v>30.8130068485406</v>
       </c>
       <c r="F28" t="n">
-        <v>0.9819807771634412</v>
+        <v>0.2435943369744775</v>
       </c>
       <c r="G28" t="n">
-        <v>0.005357277341859056</v>
+        <v>0.008307420860468345</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0001108832397313734</v>
+        <v>6.567488484394946e-05</v>
       </c>
       <c r="I28" t="n">
-        <v>0.3198856661463513</v>
+        <v>0.7796851461304722</v>
       </c>
       <c r="J28" t="n">
-        <v>0.007210493630656848</v>
+        <v>0.006212855492338484</v>
       </c>
       <c r="K28" t="n">
-        <v>1.01198905841388e-05</v>
+        <v>1.219658602695201e-05</v>
       </c>
       <c r="L28" t="n">
-        <v>0.025</v>
+        <v>0.02394557823129252</v>
       </c>
       <c r="M28" t="n">
-        <v>221.399730820996</v>
+        <v>88.81640625</v>
       </c>
       <c r="N28" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="O28" t="n">
-        <v>107</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>AC6rearSOAEwfB1.mat</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>6029.296875</v>
+        <v>4505.82275390625</v>
       </c>
       <c r="E29" t="n">
-        <v>65.18492139944397</v>
+        <v>34.91246923188895</v>
       </c>
       <c r="F29" t="n">
-        <v>1.041854192691343</v>
+        <v>1.464209079457356</v>
       </c>
       <c r="G29" t="n">
-        <v>0.01081136370473447</v>
+        <v>0.007748300618709901</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0001727986221762124</v>
+        <v>0.0003249593158514688</v>
       </c>
       <c r="I29" t="n">
-        <v>0.1594845186078768</v>
+        <v>0.2233787296692884</v>
       </c>
       <c r="J29" t="n">
-        <v>0.002372531664334035</v>
+        <v>0.01102984299433275</v>
       </c>
       <c r="K29" t="n">
-        <v>3.586525224037378e-06</v>
+        <v>2.232136437705074e-05</v>
       </c>
       <c r="L29" t="n">
-        <v>0.03192743764172336</v>
+        <v>0.02893424036281179</v>
       </c>
       <c r="M29" t="n">
-        <v>192.5</v>
+        <v>130.37255859375</v>
       </c>
       <c r="N29" t="n">
         <v>6</v>
       </c>
       <c r="O29" t="n">
-        <v>85</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>ACsb4rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>8101.86767578125</v>
+        <v>963.61083984375</v>
       </c>
       <c r="E30" t="n">
-        <v>43.16336482283502</v>
+        <v>13.95337452751453</v>
       </c>
       <c r="F30" t="n">
-        <v>0.6319865427086913</v>
+        <v>0.2930260777259106</v>
       </c>
       <c r="G30" t="n">
-        <v>0.005327582052699083</v>
+        <v>0.01448030050157704</v>
       </c>
       <c r="H30" t="n">
-        <v>7.800504377501448e-05</v>
+        <v>0.0003040917200282065</v>
       </c>
       <c r="I30" t="n">
-        <v>0.2330811980465607</v>
+        <v>0.2562669913717123</v>
       </c>
       <c r="J30" t="n">
-        <v>0.003655142612314343</v>
+        <v>0.00527925178374748</v>
       </c>
       <c r="K30" t="n">
-        <v>2.283939076446799e-06</v>
+        <v>1.973086627418672e-05</v>
       </c>
       <c r="L30" t="n">
-        <v>0.01795918367346939</v>
+        <v>0.04390022675736961</v>
       </c>
       <c r="M30" t="n">
-        <v>145.5029296875</v>
+        <v>42.302734375</v>
       </c>
       <c r="N30" t="n">
         <v>6</v>
       </c>
       <c r="O30" t="n">
-        <v>103</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>TAG6rearSOAEwf1.mat</t>
+          <t>ACsb4rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>9856.82373046875</v>
+        <v>3154.6142578125</v>
       </c>
       <c r="E31" t="n">
-        <v>67.29629674226393</v>
+        <v>23.78540061610909</v>
       </c>
       <c r="F31" t="n">
-        <v>1.129070389633301</v>
+        <v>0.5264083942706108</v>
       </c>
       <c r="G31" t="n">
-        <v>0.006827381576708342</v>
+        <v>0.0075398760901444</v>
       </c>
       <c r="H31" t="n">
-        <v>0.0001145470813425622</v>
+        <v>0.0001668693384514269</v>
       </c>
       <c r="I31" t="n">
-        <v>0.1483513657837621</v>
+        <v>0.5805720080050166</v>
       </c>
       <c r="J31" t="n">
-        <v>0.002379053373154873</v>
+        <v>0.01507727675807756</v>
       </c>
       <c r="K31" t="n">
-        <v>1.731241847679568e-06</v>
+        <v>3.471694046130892e-05</v>
       </c>
       <c r="L31" t="n">
-        <v>0.01895691609977324</v>
+        <v>0.02394557823129252</v>
       </c>
       <c r="M31" t="n">
-        <v>186.85498046875</v>
+        <v>75.5390625</v>
       </c>
       <c r="N31" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="O31" t="n">
-        <v>113</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Owl</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>TAG9rearSOAEwf2.mat</t>
+          <t>ACsb4rearSOAEwf1.mat</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>6976.7578125</v>
+        <v>3951.3427734375</v>
       </c>
       <c r="E32" t="n">
-        <v>62.31430300866985</v>
+        <v>23.63591322506127</v>
       </c>
       <c r="F32" t="n">
-        <v>2.242419058195079</v>
+        <v>1.213516406693819</v>
       </c>
       <c r="G32" t="n">
-        <v>0.008931699319850777</v>
+        <v>0.005981742050816572</v>
       </c>
       <c r="H32" t="n">
-        <v>0.0003214127705819771</v>
+        <v>0.0003071149420018833</v>
       </c>
       <c r="I32" t="n">
-        <v>0.4420795635573023</v>
+        <v>0.3166557606045285</v>
       </c>
       <c r="J32" t="n">
-        <v>0.01627421036470345</v>
+        <v>0.01407616308989853</v>
       </c>
       <c r="K32" t="n">
-        <v>0.0001260786954649355</v>
+        <v>8.442922690377912e-05</v>
       </c>
       <c r="L32" t="n">
-        <v>0.09977324263038549</v>
+        <v>0.01696145124716553</v>
       </c>
       <c r="M32" t="n">
-        <v>696.09375</v>
+        <v>67.0205078125</v>
       </c>
       <c r="N32" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O32" t="n">
-        <v>73</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ALrearSOAEwf1.mat</t>
+          <t>ACsb24rearSOAEwfA1.mat</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>2804.69970703125</v>
+        <v>2174.853515625</v>
       </c>
       <c r="E33" t="n">
-        <v>188.1689563901322</v>
+        <v>22.67144366060593</v>
       </c>
       <c r="F33" t="n">
-        <v>2.207577677156686</v>
+        <v>0.2476911360366756</v>
       </c>
       <c r="G33" t="n">
-        <v>0.06709058938409751</v>
+        <v>0.0104243543290274</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0007870994786437894</v>
+        <v>0.0001138886523883863</v>
       </c>
       <c r="I33" t="n">
-        <v>0.4818796976081177</v>
+        <v>0.8791720462483861</v>
       </c>
       <c r="J33" t="n">
-        <v>0.005459584270559902</v>
+        <v>0.009760100231312211</v>
       </c>
       <c r="K33" t="n">
-        <v>9.741184714092239e-05</v>
+        <v>3.722065890161057e-05</v>
       </c>
       <c r="L33" t="n">
-        <v>0.1825850340136054</v>
+        <v>0.02993197278911565</v>
       </c>
       <c r="M33" t="n">
-        <v>512.09619140625</v>
+        <v>65.09765625</v>
       </c>
       <c r="N33" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="O33" t="n">
-        <v>13</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ALrearSOAEwf1.mat</t>
+          <t>ACsb24rearSOAEwfA1.mat</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>2944.66552734375</v>
+        <v>2503.23486328125</v>
       </c>
       <c r="E34" t="n">
-        <v>207.6946572753118</v>
+        <v>22.40099039650308</v>
       </c>
       <c r="F34" t="n">
-        <v>2.191252810388788</v>
+        <v>0.256295236792185</v>
       </c>
       <c r="G34" t="n">
-        <v>0.07053251221460922</v>
+        <v>0.008948816878948294</v>
       </c>
       <c r="H34" t="n">
-        <v>0.0007441431938673925</v>
+        <v>0.0001023856133324351</v>
       </c>
       <c r="I34" t="n">
-        <v>0.6952234852094058</v>
+        <v>0.7858689253863718</v>
       </c>
       <c r="J34" t="n">
-        <v>0.006869531748911356</v>
+        <v>0.008895026709165666</v>
       </c>
       <c r="K34" t="n">
-        <v>0.0002213060140282346</v>
+        <v>3.152883977299496e-05</v>
       </c>
       <c r="L34" t="n">
-        <v>0.2244897959183673</v>
+        <v>0.02693877551020408</v>
       </c>
       <c r="M34" t="n">
-        <v>661.04736328125</v>
+        <v>67.43408203125</v>
       </c>
       <c r="N34" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O34" t="n">
-        <v>13</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ALrearSOAEwf1.mat</t>
+          <t>ACsb24rearSOAEwfA1.mat</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>3865.2099609375</v>
+        <v>3111.5478515625</v>
       </c>
       <c r="E35" t="n">
-        <v>317.0183394985274</v>
+        <v>21.10718693998504</v>
       </c>
       <c r="F35" t="n">
-        <v>1.224955420503362</v>
+        <v>0.3278849505140523</v>
       </c>
       <c r="G35" t="n">
-        <v>0.08201840073433815</v>
+        <v>0.006783500671341379</v>
       </c>
       <c r="H35" t="n">
-        <v>0.0003169182095883483</v>
+        <v>0.000105376798351149</v>
       </c>
       <c r="I35" t="n">
-        <v>0.7315637542423631</v>
+        <v>0.6343833786836998</v>
       </c>
       <c r="J35" t="n">
-        <v>0.002627587894898712</v>
+        <v>0.01089729202042138</v>
       </c>
       <c r="K35" t="n">
-        <v>4.560392155104465e-05</v>
+        <v>2.210011525325792e-05</v>
       </c>
       <c r="L35" t="n">
-        <v>0.3901133786848073</v>
+        <v>0.02195011337868481</v>
       </c>
       <c r="M35" t="n">
-        <v>1507.8701171875</v>
+        <v>68.298828125</v>
       </c>
       <c r="N35" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="O35" t="n">
-        <v>13</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>JIrearSOAEwf2.mat</t>
+          <t>ACsb24rearSOAEwfA1.mat</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>2341.73583984375</v>
+        <v>3477.6123046875</v>
       </c>
       <c r="E36" t="n">
-        <v>552.0015147115423</v>
+        <v>26.39986895585885</v>
       </c>
       <c r="F36" t="n">
-        <v>4.085849135693317</v>
+        <v>0.3180161390595472</v>
       </c>
       <c r="G36" t="n">
-        <v>0.2357232209199027</v>
+        <v>0.007591377831356954</v>
       </c>
       <c r="H36" t="n">
-        <v>0.001744795064487693</v>
+        <v>9.144669134937521e-05</v>
       </c>
       <c r="I36" t="n">
-        <v>1.132929212234927</v>
+        <v>0.5163008724799766</v>
       </c>
       <c r="J36" t="n">
-        <v>0.006062085315000938</v>
+        <v>0.007269669071100952</v>
       </c>
       <c r="K36" t="n">
-        <v>0.001085336212391207</v>
+        <v>8.219741236052716e-06</v>
       </c>
       <c r="L36" t="n">
-        <v>0.4998639455782313</v>
+        <v>0.02394557823129252</v>
       </c>
       <c r="M36" t="n">
-        <v>1170.54931640625</v>
+        <v>83.2734375</v>
       </c>
       <c r="N36" t="n">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="O36" t="n">
-        <v>13</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>JIrearSOAEwf2.mat</t>
+          <t>ACsb30learSOAEwfA2.mat</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>4048.2421875</v>
+        <v>1798.0224609375</v>
       </c>
       <c r="E37" t="n">
-        <v>551.3635391031806</v>
+        <v>13.85107494932291</v>
       </c>
       <c r="F37" t="n">
-        <v>4.833585760431367</v>
+        <v>0.2662793309785116</v>
       </c>
       <c r="G37" t="n">
-        <v>0.1361982592853903</v>
+        <v>0.007703504961835057</v>
       </c>
       <c r="H37" t="n">
-        <v>0.001193996193052955</v>
+        <v>0.0001480956644110396</v>
       </c>
       <c r="I37" t="n">
-        <v>1.157471109475048</v>
+        <v>0.5708268880197924</v>
       </c>
       <c r="J37" t="n">
-        <v>0.009938885453286481</v>
+        <v>0.01155023624929404</v>
       </c>
       <c r="K37" t="n">
-        <v>0.0008080794932110592</v>
+        <v>3.647036017229433e-05</v>
       </c>
       <c r="L37" t="n">
-        <v>0.4998639455782313</v>
+        <v>0.02494331065759637</v>
       </c>
       <c r="M37" t="n">
-        <v>2023.5703125</v>
+        <v>44.8486328125</v>
       </c>
       <c r="N37" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="O37" t="n">
-        <v>10</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Anole</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>JIrearSOAEwf2.mat</t>
+          <t>ACsb30learSOAEwfA2.mat</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>5840.88134765625</v>
+        <v>2142.5537109375</v>
       </c>
       <c r="E38" t="n">
-        <v>462.5191503790483</v>
+        <v>9.363137082035923</v>
       </c>
       <c r="F38" t="n">
-        <v>5.472510926017992</v>
+        <v>0.3226959282252587</v>
       </c>
       <c r="G38" t="n">
-        <v>0.07918653416314332</v>
+        <v>0.004370082782166974</v>
       </c>
       <c r="H38" t="n">
-        <v>0.0009369323908991795</v>
+        <v>0.0001506127601739605</v>
       </c>
       <c r="I38" t="n">
-        <v>0.758518707623195</v>
+        <v>0.2479408997732833</v>
       </c>
       <c r="J38" t="n">
-        <v>0.008720826950622306</v>
+        <v>0.009945666432332079</v>
       </c>
       <c r="K38" t="n">
-        <v>0.0003426250567257993</v>
+        <v>8.995472667836697e-06</v>
       </c>
       <c r="L38" t="n">
-        <v>0.254421768707483</v>
+        <v>0.01496598639455782</v>
       </c>
       <c r="M38" t="n">
-        <v>1486.04736328125</v>
+        <v>32.0654296875</v>
       </c>
       <c r="N38" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="O38" t="n">
-        <v>12</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>LSrearSOAEwf1.mat</t>
+          <t>tokay_GG1rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>732.12890625</v>
+        <v>1571.923828125</v>
       </c>
       <c r="E39" t="n">
-        <v>-732.12890625</v>
+        <v>19.44893149240678</v>
       </c>
       <c r="F39" t="n">
-        <v>-732.12890625</v>
+        <v>0.764489709378775</v>
       </c>
       <c r="G39" t="n">
-        <v>-1</v>
+        <v>0.0123726933483829</v>
       </c>
       <c r="H39" t="n">
-        <v>-1</v>
+        <v>0.0004863401748230147</v>
       </c>
       <c r="I39" t="n">
-        <v>-1</v>
+        <v>0.2241610255845824</v>
       </c>
       <c r="J39" t="n">
-        <v>-1</v>
+        <v>0.01000480619777373</v>
       </c>
       <c r="K39" t="n">
-        <v>-1</v>
+        <v>3.905384820143816e-05</v>
       </c>
       <c r="L39" t="n">
-        <v>0.00199546485260771</v>
+        <v>0.05387755102040816</v>
       </c>
       <c r="M39" t="n">
-        <v>1.4609375</v>
-      </c>
-      <c r="N39" t="n">
-        <v>10</v>
-      </c>
-      <c r="O39" t="n">
-        <v>5</v>
-      </c>
+        <v>84.69140625</v>
+      </c>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>LSrearSOAEwf1.mat</t>
+          <t>tokay_GG2rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>985.14404296875</v>
+        <v>3176.1474609375</v>
       </c>
       <c r="E40" t="n">
-        <v>-985.14404296875</v>
+        <v>32.85341980531391</v>
       </c>
       <c r="F40" t="n">
-        <v>-985.14404296875</v>
+        <v>0.4692634639329732</v>
       </c>
       <c r="G40" t="n">
-        <v>-1</v>
+        <v>0.01034379549733393</v>
       </c>
       <c r="H40" t="n">
-        <v>-1</v>
+        <v>0.0001477461200099511</v>
       </c>
       <c r="I40" t="n">
-        <v>-1</v>
+        <v>0.3844365974395721</v>
       </c>
       <c r="J40" t="n">
-        <v>-1</v>
+        <v>0.005160778550214174</v>
       </c>
       <c r="K40" t="n">
-        <v>-1</v>
+        <v>1.507532083469712e-05</v>
       </c>
       <c r="L40" t="n">
-        <v>0.0009977324263038549</v>
+        <v>0.02993197278911565</v>
       </c>
       <c r="M40" t="n">
-        <v>0.9829101562500001</v>
-      </c>
-      <c r="N40" t="n">
-        <v>10</v>
-      </c>
-      <c r="O40" t="n">
-        <v>5</v>
-      </c>
+        <v>95.068359375</v>
+      </c>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -2474,101 +2502,93 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>LSrearSOAEwf1.mat</t>
+          <t>tokay_GG3rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2228.6865234375</v>
+        <v>1108.9599609375</v>
       </c>
       <c r="E41" t="n">
-        <v>338.668751015891</v>
+        <v>18.07021742352932</v>
       </c>
       <c r="F41" t="n">
-        <v>2.892077659109331</v>
+        <v>0.2155644170633567</v>
       </c>
       <c r="G41" t="n">
-        <v>0.1519588993132746</v>
+        <v>0.01629474287624685</v>
       </c>
       <c r="H41" t="n">
-        <v>0.00129766013689921</v>
+        <v>0.0001943843102154215</v>
       </c>
       <c r="I41" t="n">
-        <v>1.115416307619816</v>
+        <v>0.2111880641374601</v>
       </c>
       <c r="J41" t="n">
-        <v>0.009586979254335498</v>
+        <v>0.002515092212367823</v>
       </c>
       <c r="K41" t="n">
-        <v>0.000693938966408099</v>
+        <v>4.732434660352584e-06</v>
       </c>
       <c r="L41" t="n">
-        <v>0.4998639455782313</v>
+        <v>0.04988662131519275</v>
       </c>
       <c r="M41" t="n">
-        <v>1114.0400390625</v>
-      </c>
-      <c r="N41" t="n">
-        <v>15</v>
-      </c>
-      <c r="O41" t="n">
-        <v>7</v>
-      </c>
+        <v>55.322265625</v>
+      </c>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>TH13RearwaveformSOAE.mat</t>
+          <t>tokay_GG3rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>904.39453125</v>
+        <v>3133.0810546875</v>
       </c>
       <c r="E42" t="n">
-        <v>210.9332394915441</v>
+        <v>31.55561451691447</v>
       </c>
       <c r="F42" t="n">
-        <v>0.7685158465268485</v>
+        <v>0.9330798169836585</v>
       </c>
       <c r="G42" t="n">
-        <v>0.2332314407076354</v>
+        <v>0.01007175172493643</v>
       </c>
       <c r="H42" t="n">
-        <v>0.0008497572906203357</v>
+        <v>0.0002978154093995266</v>
       </c>
       <c r="I42" t="n">
-        <v>0.8304849146784853</v>
+        <v>0.2890700675077088</v>
       </c>
       <c r="J42" t="n">
-        <v>0.002884211023953616</v>
+        <v>0.007985623938169893</v>
       </c>
       <c r="K42" t="n">
-        <v>6.446261746317444e-05</v>
+        <v>3.217859291392112e-05</v>
       </c>
       <c r="L42" t="n">
-        <v>0.4998639455782313</v>
+        <v>0.02693877551020408</v>
       </c>
       <c r="M42" t="n">
-        <v>452.07421875</v>
-      </c>
-      <c r="N42" t="n">
-        <v>12</v>
-      </c>
-      <c r="O42" t="n">
-        <v>8</v>
-      </c>
+        <v>84.4013671875</v>
+      </c>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -2576,50 +2596,46 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>TH13RearwaveformSOAE.mat</t>
+          <t>tokay_GG4rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>1518.0908203125</v>
+        <v>1103.57666015625</v>
       </c>
       <c r="E43" t="n">
-        <v>421.4164440721261</v>
+        <v>16.48453568243034</v>
       </c>
       <c r="F43" t="n">
-        <v>2.090463066516357</v>
+        <v>0.2362426645157864</v>
       </c>
       <c r="G43" t="n">
-        <v>0.2775963324680254</v>
+        <v>0.01493737252480165</v>
       </c>
       <c r="H43" t="n">
-        <v>0.001377034258125633</v>
+        <v>0.0002140700080430642</v>
       </c>
       <c r="I43" t="n">
-        <v>0.9241584965480868</v>
+        <v>0.2652996395485779</v>
       </c>
       <c r="J43" t="n">
-        <v>0.003459231274733873</v>
+        <v>0.003634188822207645</v>
       </c>
       <c r="K43" t="n">
-        <v>0.0002330808561575681</v>
+        <v>9.578602028146143e-06</v>
       </c>
       <c r="L43" t="n">
-        <v>0.4998639455782313</v>
+        <v>0.04090702947845805</v>
       </c>
       <c r="M43" t="n">
-        <v>758.8388671875</v>
-      </c>
-      <c r="N43" t="n">
-        <v>14</v>
-      </c>
-      <c r="O43" t="n">
-        <v>12</v>
-      </c>
+        <v>45.14404296875</v>
+      </c>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -2627,50 +2643,46 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>TH13RearwaveformSOAE.mat</t>
+          <t>tokay_GG4rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>2040.27099609375</v>
+        <v>2287.90283203125</v>
       </c>
       <c r="E44" t="n">
-        <v>267.9062395225522</v>
+        <v>24.76979171074164</v>
       </c>
       <c r="F44" t="n">
-        <v>1.558497173643926</v>
+        <v>0.4018126750668053</v>
       </c>
       <c r="G44" t="n">
-        <v>0.1313091447339488</v>
+        <v>0.01082641769744674</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0007638677296436524</v>
+        <v>0.0001756248864424313</v>
       </c>
       <c r="I44" t="n">
-        <v>0.9641389931917534</v>
+        <v>0.2204680716251192</v>
       </c>
       <c r="J44" t="n">
-        <v>0.00475279829205009</v>
+        <v>0.003643616655424199</v>
       </c>
       <c r="K44" t="n">
-        <v>0.0003361401639476772</v>
+        <v>6.147625983686359e-06</v>
       </c>
       <c r="L44" t="n">
-        <v>0.4998639455782313</v>
+        <v>0.03492063492063492</v>
       </c>
       <c r="M44" t="n">
-        <v>1019.85791015625</v>
-      </c>
-      <c r="N44" t="n">
-        <v>17</v>
-      </c>
-      <c r="O44" t="n">
-        <v>14</v>
-      </c>
+        <v>79.89501953125</v>
+      </c>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Tokay</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -2678,233 +2690,41 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>TH13RearwaveformSOAE.mat</t>
+          <t>tokay_GG4rearSOAEwf.mat</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>2697.03369140625</v>
+        <v>3159.99755859375</v>
       </c>
       <c r="E45" t="n">
-        <v>111.2000173126638</v>
+        <v>26.20831023827449</v>
       </c>
       <c r="F45" t="n">
-        <v>1.024908800180727</v>
+        <v>0.8326714209190555</v>
       </c>
       <c r="G45" t="n">
-        <v>0.04123048876511567</v>
+        <v>0.008293775470490431</v>
       </c>
       <c r="H45" t="n">
-        <v>0.000380013347051046</v>
+        <v>0.0002635038177971276</v>
       </c>
       <c r="I45" t="n">
-        <v>0.191561897263573</v>
+        <v>0.2485909046910533</v>
       </c>
       <c r="J45" t="n">
-        <v>0.001313430264386234</v>
+        <v>0.00712889304454184</v>
       </c>
       <c r="K45" t="n">
-        <v>2.761927621449018e-06</v>
+        <v>2.542478892194142e-05</v>
       </c>
       <c r="L45" t="n">
-        <v>0.061859410430839</v>
+        <v>0.02294784580498866</v>
       </c>
       <c r="M45" t="n">
-        <v>166.8369140625</v>
-      </c>
-      <c r="N45" t="n">
-        <v>6</v>
-      </c>
-      <c r="O45" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>V Sim Human</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>0</v>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>longMCsoaeL1_20dBdiff100dB_InpN1InpYN0gain85R1rs43.mat</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>1157.469717362046</v>
-      </c>
-      <c r="E46" t="n">
-        <v>25.70684209636975</v>
-      </c>
-      <c r="F46" t="n">
-        <v>0.2403800457828528</v>
-      </c>
-      <c r="G46" t="n">
-        <v>0.02220951590418921</v>
-      </c>
-      <c r="H46" t="n">
-        <v>0.0002076771790891391</v>
-      </c>
-      <c r="I46" t="n">
-        <v>0.291023679862827</v>
-      </c>
-      <c r="J46" t="n">
-        <v>0.002995621268138478</v>
-      </c>
-      <c r="K46" t="n">
-        <v>5.823161247163234e-06</v>
-      </c>
-      <c r="L46" t="n">
-        <v>0.068</v>
-      </c>
-      <c r="M46" t="n">
-        <v>78.70794078061911</v>
-      </c>
-      <c r="N46" t="inlineStr"/>
-      <c r="O46" t="inlineStr"/>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>V Sim Human</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>0</v>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>longMCsoaeL1_20dBdiff100dB_InpN1InpYN0gain85R1rs43.mat</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>1243.606998654105</v>
-      </c>
-      <c r="E47" t="n">
-        <v>33.31379215714709</v>
-      </c>
-      <c r="F47" t="n">
-        <v>0.3274326216906659</v>
-      </c>
-      <c r="G47" t="n">
-        <v>0.02678803849865832</v>
-      </c>
-      <c r="H47" t="n">
-        <v>0.0002632926817274511</v>
-      </c>
-      <c r="I47" t="n">
-        <v>0.463610390320812</v>
-      </c>
-      <c r="J47" t="n">
-        <v>0.004931144970475302</v>
-      </c>
-      <c r="K47" t="n">
-        <v>2.579555025014002e-05</v>
-      </c>
-      <c r="L47" t="n">
-        <v>0.111</v>
-      </c>
-      <c r="M47" t="n">
-        <v>138.0403768506056</v>
-      </c>
-      <c r="N47" t="inlineStr"/>
-      <c r="O47" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>V Sim Human</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>longMCsoaeL1_20dBdiff100dB_InpN1InpYN0gain85R1rs43.mat</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>1518.169582772544</v>
-      </c>
-      <c r="E48" t="n">
-        <v>49.72888662082999</v>
-      </c>
-      <c r="F48" t="n">
-        <v>1.977855538182568</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0.03275581804900415</v>
-      </c>
-      <c r="H48" t="n">
-        <v>0.001302789596515645</v>
-      </c>
-      <c r="I48" t="n">
-        <v>0.07756935254816746</v>
-      </c>
-      <c r="J48" t="n">
-        <v>0.002115482363259324</v>
-      </c>
-      <c r="K48" t="n">
-        <v>9.009155360984471e-07</v>
-      </c>
-      <c r="L48" t="n">
-        <v>0.033</v>
-      </c>
-      <c r="M48" t="n">
-        <v>50.09959623149394</v>
-      </c>
-      <c r="N48" t="inlineStr"/>
-      <c r="O48" t="inlineStr"/>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>V Sim Human</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>0</v>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>longMCsoaeL1_20dBdiff100dB_InpN1InpYN0gain85R1rs43.mat</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>1975.773889636608</v>
-      </c>
-      <c r="E49" t="n">
-        <v>283.8268922167093</v>
-      </c>
-      <c r="F49" t="n">
-        <v>3.231228875057588</v>
-      </c>
-      <c r="G49" t="n">
-        <v>0.1436535292350239</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0.001635424423820019</v>
-      </c>
-      <c r="I49" t="n">
-        <v>0.8135707178361609</v>
-      </c>
-      <c r="J49" t="n">
-        <v>0.006156821790184477</v>
-      </c>
-      <c r="K49" t="n">
-        <v>0.0003138779271232366</v>
-      </c>
-      <c r="L49" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="M49" t="n">
-        <v>395.1547779273217</v>
-      </c>
-      <c r="N49" t="inlineStr"/>
-      <c r="O49" t="inlineStr"/>
+        <v>72.51513671875</v>
+      </c>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>